<commit_message>
Updated Config Properties to include the Output File Path
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Output.xlsx
+++ b/On-Call-Tracker/src/inputs/Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,6 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -410,24 +411,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.83203125"/>
+    <col min="5" max="5" customWidth="true" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SupplyTeacherList and Reader
Added Supply Teacher List excel file and the reader
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Output.xlsx
+++ b/On-Call-Tracker/src/inputs/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ED86731-5C27-3B43-AF3E-D85DD21F1901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761D31F7-010E-1445-8939-ECE5807FD8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34900" yWindow="2740" windowWidth="28040" windowHeight="16080" xr2:uid="{3850AB85-AA1A-CB4A-92DC-B712A94A710D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>Day</t>
   </si>
@@ -65,18 +65,12 @@
     <t>SBI3U</t>
   </si>
   <si>
-    <t>Angela Griffith</t>
-  </si>
-  <si>
     <t>FEF1D</t>
   </si>
   <si>
     <t>ICS2O</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Fletcher Donaldson</t>
   </si>
   <si>
@@ -86,10 +80,31 @@
     <t>Gloria Grewal</t>
   </si>
   <si>
+    <t>Lori Pearson</t>
+  </si>
+  <si>
     <t>Leigh Atkinson</t>
   </si>
   <si>
-    <t>Lori Pearson</t>
+    <t>Matt Gates</t>
+  </si>
+  <si>
+    <t>Mustapha Chamorro</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Dineth</t>
+  </si>
+  <si>
+    <t>Marno</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Abdel</t>
   </si>
 </sst>
 </file>
@@ -97,8 +112,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,13 +149,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -143,6 +186,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA199561-44DC-F742-9EDF-21A24A41F2FB}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E28" xr:uid="{CA199561-44DC-F742-9EDF-21A24A41F2FB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{528E8620-9D96-E840-A1B7-F0FCEB8F318A}" name="Day"/>
+    <tableColumn id="2" xr3:uid="{4550AC7B-EED0-6140-A024-CB8313D61A15}" name="Absentee Period"/>
+    <tableColumn id="3" xr3:uid="{A0605465-7096-0D41-A067-3F5C6B6538F8}" name="Subject"/>
+    <tableColumn id="4" xr3:uid="{17541AF9-37BD-0C47-97BF-4908044E70D4}" name="Supply"/>
+    <tableColumn id="5" xr3:uid="{545CAEA0-1FC6-CA4E-BDBE-428F79A5A70B}" name="Replacement"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,29 +502,29 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="15.83203125"/>
+    <col min="2" max="2" customWidth="true" width="16.83203125"/>
     <col min="5" max="5" customWidth="true" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -482,10 +539,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -499,10 +556,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -513,13 +570,13 @@
         <v>3.0</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -530,17 +587,20 @@
         <v>1.0</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Printouts to OnCall
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Output.xlsx
+++ b/On-Call-Tracker/src/inputs/Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Day</t>
   </si>
@@ -96,12 +96,31 @@
   </si>
   <si>
     <t>Absentee ID</t>
+  </si>
+  <si>
+    <t>Abigail Hays</t>
+  </si>
+  <si>
+    <t>Alfred Perry</t>
+  </si>
+  <si>
+    <t>HRE2OF-01</t>
+  </si>
+  <si>
+    <t>Amanda Bush</t>
+  </si>
+  <si>
+    <t>Bobbi Fletcher</t>
+  </si>
+  <si>
+    <t>Fletcher Donaldson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -492,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29535FD7-6A1F-B748-AEBC-E925AC52ED71}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
@@ -500,11 +519,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="16.83203125"/>
+    <col min="5" max="5" customWidth="true" width="16.5"/>
+    <col min="6" max="6" customWidth="true" width="17.1640625"/>
+    <col min="7" max="7" customWidth="true" width="16.1640625"/>
+    <col min="8" max="8" customWidth="true" width="18.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -533,91 +552,163 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="n">
+        <v>165.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100.0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="n">
+        <v>165.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
+      <c r="F4" t="n">
+        <v>166.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="n">
+        <v>102.0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="n">
+        <v>165.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="n">
+        <v>104.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="n">
+        <v>166.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="n">
+        <v>107.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
+      <c r="F7" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="n">
+        <v>120.0</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="8"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>